<commit_message>
Alterações nos arquivos tabelas e modelo lógico
</commit_message>
<xml_diff>
--- a/tabelas.xlsx
+++ b/tabelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>id_cliente</t>
   </si>
@@ -305,10 +305,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -316,9 +319,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -601,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,11 +634,6 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -651,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -678,7 +673,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -687,32 +682,32 @@
       <c r="C2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="8"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="9"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -721,13 +716,13 @@
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>51</v>
       </c>
       <c r="L5" s="3"/>
@@ -738,13 +733,13 @@
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="5" t="s">
         <v>52</v>
       </c>
       <c r="L6" s="3"/>
@@ -752,16 +747,16 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>53</v>
       </c>
       <c r="L7" s="3"/>
@@ -769,29 +764,29 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="9"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L9" s="3"/>
@@ -799,60 +794,60 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -860,52 +855,52 @@
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D16:D17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1262,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alteracoes nos arquivos logico.png e tabelas
</commit_message>
<xml_diff>
--- a/tabelas.xlsx
+++ b/tabelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>id_cliente</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Tabela para cadastro e informações de pedidos de fornecedores.</t>
+  </si>
+  <si>
+    <t>produto</t>
+  </si>
+  <si>
+    <t>tipo</t>
   </si>
 </sst>
 </file>
@@ -309,9 +315,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -320,6 +323,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,7 +679,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -682,32 +688,32 @@
       <c r="C2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="7"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="8"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -747,7 +753,7 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -756,7 +762,7 @@
       <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>53</v>
       </c>
       <c r="L7" s="3"/>
@@ -764,20 +770,20 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="8"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -786,7 +792,7 @@
       <c r="C9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>50</v>
       </c>
       <c r="L9" s="3"/>
@@ -794,17 +800,17 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -813,29 +819,29 @@
       <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -866,7 +872,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -875,32 +881,32 @@
       <c r="C16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1010,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1044,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1048,11 +1054,16 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1257,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Últimas alterações no modelo lógico e no arquivo tabelas
</commit_message>
<xml_diff>
--- a/tabelas.xlsx
+++ b/tabelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>id_cliente</t>
   </si>
@@ -74,9 +74,6 @@
     <t>nome_contato</t>
   </si>
   <si>
-    <t>observação</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>id_prod</t>
   </si>
   <si>
-    <t>tipo_prod</t>
-  </si>
-  <si>
     <t>qtd_prod</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>nome_fornecedor</t>
   </si>
   <si>
-    <t>*id_produto</t>
-  </si>
-  <si>
     <t>Entidade</t>
   </si>
   <si>
@@ -210,6 +201,12 @@
   </si>
   <si>
     <t>tipo</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>prod</t>
   </si>
 </sst>
 </file>
@@ -315,6 +312,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -323,9 +323,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -640,7 +637,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -666,70 +663,70 @@
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="D3" s="8"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="D4" s="9"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -737,176 +734,176 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>36</v>
+      <c r="A7" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="8"/>
+        <v>43</v>
+      </c>
+      <c r="D8" s="9"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>37</v>
+      <c r="A9" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>56</v>
+      <c r="D16" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="D17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D16:D17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -996,7 +993,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1016,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,32 +1036,37 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1087,27 +1089,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1117,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1132,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1151,11 +1153,6 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1183,7 +1180,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1193,7 +1190,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1221,7 +1218,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1246,7 +1243,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1266,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,32 +1281,37 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>